<commit_message>
PACKAGE INSERTS TABLAS II
ENCABEZADO - BODY
MARIELA
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/Casos de Prueba.xlsx
+++ b/DOCUMENTACION/Casos de Prueba.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{220A882C-DB48-48D3-A4C9-51DF167B7CF2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7DB23F80-9B7D-474C-86DD-9FF0BF7891AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="45">
   <si>
     <t>Id</t>
   </si>
@@ -65,6 +66,96 @@
   </si>
   <si>
     <t>Inscribirse en una actividad</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>package body</t>
+  </si>
+  <si>
+    <t>triggers</t>
+  </si>
+  <si>
+    <t>insert</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>ACTIVIDAD</t>
+  </si>
+  <si>
+    <t>AXP</t>
+  </si>
+  <si>
+    <t>BIRACORA AXP</t>
+  </si>
+  <si>
+    <t>BITACORA USUARIO</t>
+  </si>
+  <si>
+    <t>CANTON</t>
+  </si>
+  <si>
+    <t>CONTACTO EMERGENCIA</t>
+  </si>
+  <si>
+    <t>CORREO</t>
+  </si>
+  <si>
+    <t>DISTRITO</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>EVENTO</t>
+  </si>
+  <si>
+    <t>INSTITUCION</t>
+  </si>
+  <si>
+    <t>NACIONALIDAD</t>
+  </si>
+  <si>
+    <t>OCUPACION</t>
+  </si>
+  <si>
+    <t>PAIS</t>
+  </si>
+  <si>
+    <t>PERSONA</t>
+  </si>
+  <si>
+    <t>PROVINCIA</t>
+  </si>
+  <si>
+    <t>TELEFONO</t>
+  </si>
+  <si>
+    <t>TIPO PARTICIPANTE</t>
+  </si>
+  <si>
+    <t>TIPO PERSONA</t>
+  </si>
+  <si>
+    <t>TIPO PUBLICO</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
+    <t>CATALOGOS</t>
+  </si>
+  <si>
+    <t>TABLAS</t>
+  </si>
+  <si>
+    <t>MARI</t>
   </si>
 </sst>
 </file>
@@ -96,15 +187,81 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -192,50 +349,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -247,6 +470,126 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -548,32 +891,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="4" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="3"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -588,10 +931,10 @@
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -605,10 +948,10 @@
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="H4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4">
         <f>+COUNTIF(E4:E53, "Pendiente")</f>
         <v>50</v>
       </c>
@@ -623,10 +966,10 @@
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="6">
         <f>+COUNTIF(E4:E54, "Con error")</f>
         <v>0</v>
       </c>
@@ -641,10 +984,10 @@
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="8">
         <f>+COUNTIF(E4:E55, "Certificado")</f>
         <v>0</v>
       </c>
@@ -1040,4 +1383,466 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A3AC1A-13A4-4AC5-A39A-5352C9801BAD}">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="4" width="8" style="11" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" style="24" customWidth="1"/>
+    <col min="6" max="8" width="8" style="11" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" style="24" customWidth="1"/>
+    <col min="10" max="11" width="8" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="F1" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
+      <c r="J1" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="47"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="39" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="50"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="F5" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="F6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="F7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="F8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="F9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="F10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="F11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="F12" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="F13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="19"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="F14" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="19"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="F15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="19"/>
+    </row>
+    <row r="16" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="50"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="F17" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="19"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="F18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="19"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="F19" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="17"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="19"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="F20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="19"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="F21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="19"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="F22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="17"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="19"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="F23" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="19"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="F24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="19"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="F25" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="17"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="19"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="F26" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A3:XFD3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CORRECIONES UPDATES - DISTRIBUCION DE TARES
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/Casos de Prueba.xlsx
+++ b/DOCUMENTACION/Casos de Prueba.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7DB23F80-9B7D-474C-86DD-9FF0BF7891AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{88491B07-9625-492F-AEEF-B0723E12BA97}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="47">
   <si>
     <t>Id</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>MARI</t>
+  </si>
+  <si>
+    <t>NAKI</t>
+  </si>
+  <si>
+    <t>IG</t>
   </si>
 </sst>
 </file>
@@ -1390,7 +1396,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F15"/>
+      <selection activeCell="A16" sqref="A16:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,15 +1474,27 @@
       <c r="B5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
+      <c r="C5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F5" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
+      <c r="G5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1485,15 +1503,27 @@
       <c r="B6" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
+      <c r="C6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="17"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19"/>
+      <c r="G6" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1502,15 +1532,27 @@
       <c r="B7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
+      <c r="C7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F7" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
+      <c r="G7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1519,15 +1561,27 @@
       <c r="B8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
+      <c r="C8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="17"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="19"/>
+      <c r="G8" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1536,15 +1590,27 @@
       <c r="B9" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
+      <c r="C9" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F9" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="G9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1553,15 +1619,27 @@
       <c r="B10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
+      <c r="C10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F10" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="17"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="G10" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1570,15 +1648,27 @@
       <c r="B11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
+      <c r="C11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F11" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="G11" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1587,15 +1677,27 @@
       <c r="B12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
+      <c r="C12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F12" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="G12" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1604,15 +1706,27 @@
       <c r="B13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
+      <c r="C13" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F13" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
+      <c r="G13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1621,15 +1735,27 @@
       <c r="B14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
+      <c r="C14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F14" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="17"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="19"/>
+      <c r="G14" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1638,15 +1764,27 @@
       <c r="B15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
+      <c r="C15" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F15" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="19"/>
+      <c r="G15" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="48" t="s">
@@ -1670,15 +1808,27 @@
       <c r="B17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
+      <c r="C17" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F17" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="19"/>
+      <c r="G17" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1687,15 +1837,27 @@
       <c r="B18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
+      <c r="C18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="G18" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1704,15 +1866,27 @@
       <c r="B19" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
+      <c r="C19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F19" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="G19" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1721,15 +1895,27 @@
       <c r="B20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
+      <c r="C20" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F20" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="17"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="G20" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1738,15 +1924,27 @@
       <c r="B21" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
+      <c r="C21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F21" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="G21" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1755,15 +1953,27 @@
       <c r="B22" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
+      <c r="C22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="16"/>
-      <c r="H22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="G22" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1772,15 +1982,27 @@
       <c r="B23" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
+      <c r="C23" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F23" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="16"/>
-      <c r="H23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="G23" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1789,15 +2011,27 @@
       <c r="B24" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
+      <c r="C24" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F24" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="17"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="19"/>
+      <c r="G24" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1806,15 +2040,27 @@
       <c r="B25" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
+      <c r="C25" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F25" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="16"/>
-      <c r="H25" s="17"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="19"/>
+      <c r="G25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1823,15 +2069,27 @@
       <c r="B26" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
+      <c r="C26" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F26" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="16"/>
-      <c r="H26" s="17"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="19"/>
+      <c r="G26" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="19" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>